<commit_message>
user : added default option & vehicule
+ some other corections on vehicule
</commit_message>
<xml_diff>
--- a/Back_end_à_faire.xlsx
+++ b/Back_end_à_faire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Projet_GLA_GPS_LIKE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6978A21E-3963-4175-A75F-4D5981995409}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEB38AE-3821-47A6-85A4-F763D1748B0E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F504AD7A-6505-4FA5-9098-C9C553E4B796}"/>
+    <workbookView xWindow="-19320" yWindow="855" windowWidth="19440" windowHeight="15000" xr2:uid="{F504AD7A-6505-4FA5-9098-C9C553E4B796}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -177,10 +177,10 @@
     <t>/suivre/:id</t>
   </si>
   <si>
-    <t>obtenir les infos d'un itinéraire</t>
-  </si>
-  <si>
     <t>UNIQUEMENT DISPONIBLE SI ON EST GESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Suivre itinéraire</t>
   </si>
 </sst>
 </file>
@@ -196,7 +196,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +206,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -222,9 +228,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,7 +549,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,16 +579,16 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -589,16 +596,16 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -771,12 +778,12 @@
         <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="1"/>
     </row>

</xml_diff>